<commit_message>
Adding ex.6 in list 4
</commit_message>
<xml_diff>
--- a/MRF17_L04.xlsx
+++ b/MRF17_L04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="7200" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11760" windowHeight="7200" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="zad4a)" sheetId="18" r:id="rId7"/>
     <sheet name="zad4b)" sheetId="19" r:id="rId8"/>
     <sheet name="zad5" sheetId="20" r:id="rId9"/>
+    <sheet name="zad6" sheetId="21" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="d" localSheetId="3">#REF!</definedName>
@@ -6260,7 +6261,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>zad3!$B$15:$B$215</c15:sqref>
@@ -6878,7 +6879,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>zad3!$F$15:$F$215</c15:sqref>
@@ -6892,7 +6893,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-179E-4D9E-9D6D-08BCC9F10F0E}"/>
                   </c:ext>
@@ -6917,7 +6918,7 @@
                 </c:marker>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>zad3!$B$15:$B$215</c15:sqref>
@@ -7535,7 +7536,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>zad3!$H$15:$H$215</c15:sqref>
@@ -7549,7 +7550,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-179E-4D9E-9D6D-08BCC9F10F0E}"/>
                   </c:ext>
@@ -8885,6 +8886,20 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
@@ -15518,7 +15533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>